<commit_message>
shift some files to backlog
</commit_message>
<xml_diff>
--- a/features/backlog/android/tools_symlexVPN.xlsx
+++ b/features/backlog/android/tools_symlexVPN.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE85A828-28F7-405C-8EC8-FA048674E54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020B5151-2E5A-4F43-B3E9-128988AE80E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -178,6 +178,13 @@
 7. Tap the"test your network"
 8. Check the "test your network" button</t>
   </si>
+  <si>
+    <t>1.The VPN app is installed and configured on the Android device.
+2. User credentials are valid.</t>
+  </si>
+  <si>
+    <t>the displayed information will accurately represents the current state of the network (IP address, server connection status).</t>
+  </si>
 </sst>
 </file>
 
@@ -250,7 +257,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -405,19 +412,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
@@ -428,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -513,9 +507,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1362,7 +1353,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1378,15 +1369,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1408,13 +1399,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1436,7 +1427,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1481,7 +1472,9 @@
       <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="31"/>
+      <c r="B4" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="C4" s="24" t="s">
         <v>13</v>
       </c>
@@ -1519,7 +1512,9 @@
       <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="C5" s="16" t="s">
         <v>18</v>
       </c>
@@ -1557,7 +1552,9 @@
       <c r="A6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="C6" s="26" t="s">
         <v>19</v>
       </c>
@@ -1595,8 +1592,10 @@
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="29" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="25" t="s">
@@ -1633,7 +1632,9 @@
       <c r="A8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="C8" s="14" t="s">
         <v>24</v>
       </c>
@@ -1671,7 +1672,9 @@
       <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="18" t="s">
         <v>33</v>
       </c>
@@ -1709,14 +1712,18 @@
       <c r="A10" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="C10" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="17" t="s">
         <v>7</v>
       </c>

</xml_diff>